<commit_message>
Key structures in progress
</commit_message>
<xml_diff>
--- a/resources/keys.xlsx
+++ b/resources/keys.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
   <si>
     <t>2. Помогает ли руководитель решать проблемные вопросы?</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>key_value</t>
+  </si>
+  <si>
+    <t>Позитивная оценка</t>
+  </si>
+  <si>
+    <t>Негативная оценка</t>
+  </si>
+  <si>
+    <t>15. Есть ли у вас функциональный руководитель? (не является руководителем по структуре, но ставит вам задачи)</t>
   </si>
 </sst>
 </file>
@@ -496,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,8 +536,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,8 +547,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,8 +558,8 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,8 +569,8 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,8 +580,8 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,8 +591,8 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,8 +602,8 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,8 +613,8 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -615,8 +624,8 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,8 +635,8 @@
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,8 +646,8 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,8 +657,8 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,8 +668,8 @@
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,8 +679,8 @@
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="C15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,8 +690,8 @@
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,8 +701,8 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,8 +712,8 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,8 +723,8 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,8 +734,8 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,8 +745,8 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,8 +756,8 @@
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="C22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,8 +767,8 @@
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="C23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,8 +778,8 @@
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24">
-        <v>0</v>
+      <c r="C24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,8 +789,8 @@
       <c r="B25" t="s">
         <v>14</v>
       </c>
-      <c r="C25">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,8 +800,8 @@
       <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="C26">
-        <v>1</v>
+      <c r="C26" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,8 +811,8 @@
       <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -813,8 +822,8 @@
       <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,8 +833,8 @@
       <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,8 +844,8 @@
       <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30">
-        <v>1</v>
+      <c r="C30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,8 +855,8 @@
       <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="C31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,8 +866,8 @@
       <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32">
-        <v>0</v>
+      <c r="C32" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,8 +877,8 @@
       <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="C33" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,8 +888,8 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34">
-        <v>1</v>
+      <c r="C34" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,8 +899,8 @@
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,8 +910,8 @@
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36">
-        <v>0</v>
+      <c r="C36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,8 +921,8 @@
       <c r="B37" t="s">
         <v>19</v>
       </c>
-      <c r="C37">
-        <v>0</v>
+      <c r="C37" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,8 +932,8 @@
       <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C38">
-        <v>1</v>
+      <c r="C38" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,8 +943,8 @@
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="C39" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,8 +954,8 @@
       <c r="B40" t="s">
         <v>8</v>
       </c>
-      <c r="C40">
-        <v>0</v>
+      <c r="C40" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,8 +965,8 @@
       <c r="B41" t="s">
         <v>41</v>
       </c>
-      <c r="C41">
-        <v>0</v>
+      <c r="C41" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,8 +976,8 @@
       <c r="B42" t="s">
         <v>32</v>
       </c>
-      <c r="C42">
-        <v>1</v>
+      <c r="C42" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,8 +987,8 @@
       <c r="B43" t="s">
         <v>33</v>
       </c>
-      <c r="C43">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,8 +998,8 @@
       <c r="B44" t="s">
         <v>34</v>
       </c>
-      <c r="C44">
-        <v>0</v>
+      <c r="C44" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,11 +1009,34 @@
       <c r="B45" t="s">
         <v>43</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>